<commit_message>
update main and support
</commit_message>
<xml_diff>
--- a/support/iCat_pinout&BOM.xlsx
+++ b/support/iCat_pinout&BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ondrej\Onekkjhvmbbvmjh Drive\Documents\GitHub\iCat\support\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OMBJ\Documents\GitHub\iCat\support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D81E85B-0C35-4EEA-8749-49FCF9F143C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3455DC6-2709-4582-85BB-03BD54692099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{22497DEB-DB2F-1D44-8AA0-0DA5ED885173}"/>
   </bookViews>
@@ -615,6 +615,67 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>250200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>278823</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Obrázek 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E1D4A5-FC0C-F124-31D1-4E92CBE7C04D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17135427" y="1073727"/>
+          <a:ext cx="5016260" cy="2809875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -921,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C95226-1D30-0842-9694-ED2035512904}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>